<commit_message>
Revert "Merge branch 'main' of github.com:Deeraniy/HX_cultural_transmission_sys"
This reverts commit 66c6d083dac7cdc1bba0a8ef1c061e5fa79cc20a, reversing
changes made to eb5a432005a76c4bbc9cb9d39f6e82d6e986bb68.
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>表名</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>comment_time</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
   </si>
   <si>
     <t>评论时间</t>
@@ -1148,8 +1151,8 @@
   <sheetPr/>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -1328,32 +1331,32 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -1364,56 +1367,56 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -1424,18 +1427,18 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -1446,7 +1449,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reapply "Merge branch 'main' of github.com:Deeraniy/HX_cultural_transmission_sys"
This reverts commit 24f833a7ef5be26493059f196dd0a76a0b1db1ba.
</commit_message>
<xml_diff>
--- a/doc/database.xlsx
+++ b/doc/database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>表名</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>comment_time</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
   </si>
   <si>
     <t>评论时间</t>
@@ -1151,8 +1148,8 @@
   <sheetPr/>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -1331,32 +1328,32 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -1367,56 +1364,56 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -1427,18 +1424,18 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -1449,7 +1446,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>